<commit_message>
Merge - Event Expense - Pages, TCs & Test Data  - 9th Oct 2025
</commit_message>
<xml_diff>
--- a/TestData/LV_T2274_VerifyValidationRulesOnEventExpense.xlsx
+++ b/TestData/LV_T2274_VerifyValidationRulesOnEventExpense.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkumar0427\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E0D4DE-924B-4193-860B-C4C600B210A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2E5057-BCF5-41DD-9F02-4134057912B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -591,7 +591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
@@ -717,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3EF9DD-8CA6-4AAD-BB71-944E6655C53E}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>